<commit_message>
Actualizacion mensaje de correo
</commit_message>
<xml_diff>
--- a/BD SUPER.xlsx
+++ b/BD SUPER.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Desktop\streamlit\rrhh_y_fact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DE9759-D389-4721-8A06-26353F3E286C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA96BCB-75E0-4127-977F-1C55A816083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{20E4A7F5-E5D8-4028-9219-BCA76ED923B4}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>SUPERVISOR TORRE</t>
   </si>
@@ -66,9 +66,6 @@
     <t>NOMBRE Y APELLIDO</t>
   </si>
   <si>
-    <t>FREDDY CASTILLO FALCON</t>
-  </si>
-  <si>
     <t>ALBIS SANCHEZ</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>ANGEL LUIS VARGAS CASTILLO</t>
+  </si>
+  <si>
+    <t>KIRA PLANCHART</t>
+  </si>
+  <si>
+    <t>SUPERVISOR ALEDAÑOS</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,6 +172,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +490,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,18 +558,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>11157858</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>20674916</v>
@@ -576,7 +580,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>15844087</v>
@@ -587,7 +591,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>19509009</v>
@@ -598,7 +602,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2">
         <v>18535738</v>
@@ -608,11 +612,11 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="A11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="2">
-        <v>10535788</v>
+        <v>16954727</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -620,7 +624,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3">
         <v>11439909</v>
@@ -631,7 +635,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
         <v>25205112</v>
@@ -642,7 +646,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
         <v>13253938</v>
@@ -653,7 +657,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <v>17078510</v>
@@ -664,46 +668,46 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>12356764</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>18930154</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>12688247</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
         <v>16576053</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>